<commit_message>
adecuar reporte para vacaciones
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
+++ b/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_retenciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979D8A86-21D0-4DEF-B688-2A8A9B76E92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F750E1-E028-48F2-8541-A1E2E62A7B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
   <si>
     <t>Empleado</t>
   </si>
@@ -30,15 +30,17 @@
   <si>
     <t>Salida</t>
   </si>
+  <si>
+    <t>Karen Burgos</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -102,7 +104,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -412,7 +414,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -439,117 +441,195 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" s="4"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10">
+        <v>45839.291666666664</v>
+      </c>
+      <c r="C2" s="10">
+        <v>45839.666666666664</v>
+      </c>
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" s="4"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="10">
+        <v>45840.291666608799</v>
+      </c>
+      <c r="C3" s="10">
+        <v>45840.666666608799</v>
+      </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" s="4"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10">
+        <v>45841.291666608799</v>
+      </c>
+      <c r="C4" s="10">
+        <v>45841.666666608799</v>
+      </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" s="4"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="10">
+        <v>45842.291666608799</v>
+      </c>
+      <c r="C5" s="10">
+        <v>45842.666666608799</v>
+      </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" s="4"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="10">
+        <v>45843.291666608799</v>
+      </c>
+      <c r="C6" s="10">
+        <v>45843.458333333336</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" s="4"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="10">
+        <v>45845.291666666664</v>
+      </c>
+      <c r="C7" s="10">
+        <v>45845.666666666664</v>
+      </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" s="4"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="10">
+        <v>45846.291666608799</v>
+      </c>
+      <c r="C8" s="10">
+        <v>45846.666666608799</v>
+      </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" s="4"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="10">
+        <v>45847.291666608799</v>
+      </c>
+      <c r="C9" s="10">
+        <v>45847.666666608799</v>
+      </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" s="4"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="10">
+        <v>45848.291666608799</v>
+      </c>
+      <c r="C10" s="10">
+        <v>45848.666666608799</v>
+      </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" s="4"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="10">
+        <v>45849.291666608799</v>
+      </c>
+      <c r="C11" s="10">
+        <v>45849.666666608799</v>
+      </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" s="4"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="10">
+        <v>45850.291666608799</v>
+      </c>
+      <c r="C12" s="10">
+        <v>45850.458333333336</v>
+      </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" s="4"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="10">
+        <v>45852.291666666664</v>
+      </c>
+      <c r="C13" s="10">
+        <v>45852.666666666664</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A14" s="4"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="10">
+        <v>45853.291666608799</v>
+      </c>
+      <c r="C14" s="10">
+        <v>45853.666666608799</v>
+      </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -591,24 +671,15 @@
       <c r="D21" s="1"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576" xr:uid="{96A1FBEE-46B7-4A65-86EA-6B887FC5B848}">
       <formula1>"Descuento,Pago normal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576" xr:uid="{D97CB041-9668-4766-9AFE-DFA262AEC773}">
+      <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D97CB041-9668-4766-9AFE-DFA262AEC773}">
-          <x14:formula1>
-            <xm:f>#REF!</xm:f>
-          </x14:formula1>
-          <xm:sqref>E1:E1048576</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Envio de recibo de nomina por correo
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
+++ b/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
@@ -8,19 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_retenciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F750E1-E028-48F2-8541-A1E2E62A7B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8842F636-8194-46D3-BC97-231CCD65EA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="7">
   <si>
     <t>Empleado</t>
   </si>
@@ -33,14 +35,24 @@
   <si>
     <t>Karen Burgos</t>
   </si>
+  <si>
+    <t>Tina Williamson</t>
+  </si>
+  <si>
+    <t>Arely siguenza</t>
+  </si>
+  <si>
+    <t>Adriana Díaz</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy\ hh:mm:ss"/>
+    <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -79,7 +91,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -100,11 +112,8 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -411,16 +420,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C14"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="16.53125" customWidth="1"/>
-    <col min="2" max="3" width="19" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="19.3984375" style="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.53125" style="2" customWidth="1"/>
     <col min="5" max="7" width="16.53125" customWidth="1"/>
   </cols>
@@ -444,10 +453,10 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>45839.291666666664</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>45839.666666666664</v>
       </c>
       <c r="D2" s="5"/>
@@ -459,11 +468,11 @@
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="10">
-        <v>45840.291666608799</v>
-      </c>
-      <c r="C3" s="10">
-        <v>45840.666666608799</v>
+      <c r="B3" s="9">
+        <v>45840.291666666664</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45840.666666666664</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
@@ -474,11 +483,11 @@
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="10">
-        <v>45841.291666608799</v>
-      </c>
-      <c r="C4" s="10">
-        <v>45841.666666608799</v>
+      <c r="B4" s="9">
+        <v>45841.291666666664</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45841.666666666664</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="6"/>
@@ -489,11 +498,11 @@
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="10">
-        <v>45842.291666608799</v>
-      </c>
-      <c r="C5" s="10">
-        <v>45842.666666608799</v>
+      <c r="B5" s="9">
+        <v>45842.291666666664</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45842.666666666664</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
@@ -504,11 +513,11 @@
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="10">
-        <v>45843.291666608799</v>
-      </c>
-      <c r="C6" s="10">
-        <v>45843.458333333336</v>
+      <c r="B6" s="9">
+        <v>45843.291666666664</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45843.666666666664</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
@@ -519,11 +528,11 @@
       <c r="A7" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="10">
-        <v>45845.291666666664</v>
-      </c>
-      <c r="C7" s="10">
-        <v>45845.666666666664</v>
+      <c r="B7" s="9">
+        <v>45844.291666666664</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45844.666666666664</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
@@ -534,11 +543,11 @@
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="10">
-        <v>45846.291666608799</v>
-      </c>
-      <c r="C8" s="10">
-        <v>45846.666666608799</v>
+      <c r="B8" s="9">
+        <v>45845.291666666664</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45845.666666666664</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
@@ -549,11 +558,11 @@
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="10">
-        <v>45847.291666608799</v>
-      </c>
-      <c r="C9" s="10">
-        <v>45847.666666608799</v>
+      <c r="B9" s="9">
+        <v>45846.291666666664</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45846.666666666664</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
@@ -564,11 +573,11 @@
       <c r="A10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="10">
-        <v>45848.291666608799</v>
-      </c>
-      <c r="C10" s="10">
-        <v>45848.666666608799</v>
+      <c r="B10" s="9">
+        <v>45847.291666666664</v>
+      </c>
+      <c r="C10" s="9">
+        <v>45847.666666666664</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
@@ -579,11 +588,11 @@
       <c r="A11" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="10">
-        <v>45849.291666608799</v>
-      </c>
-      <c r="C11" s="10">
-        <v>45849.666666608799</v>
+      <c r="B11" s="9">
+        <v>45848.291666666664</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45848.666666666664</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
@@ -594,11 +603,11 @@
       <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="10">
-        <v>45850.291666608799</v>
-      </c>
-      <c r="C12" s="10">
-        <v>45850.458333333336</v>
+      <c r="B12" s="9">
+        <v>45849.291666666664</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45849.666666666664</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
@@ -609,11 +618,11 @@
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="10">
-        <v>45852.291666666664</v>
-      </c>
-      <c r="C13" s="10">
-        <v>45852.666666666664</v>
+      <c r="B13" s="9">
+        <v>45850.291666666664</v>
+      </c>
+      <c r="C13" s="9">
+        <v>45850.666666666664</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
@@ -624,11 +633,11 @@
       <c r="A14" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="10">
-        <v>45853.291666608799</v>
-      </c>
-      <c r="C14" s="10">
-        <v>45853.666666608799</v>
+      <c r="B14" s="9">
+        <v>45851.291666666664</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45851.666666666664</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
@@ -636,39 +645,362 @@
       <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45852.291666666664</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45852.666666666664</v>
+      </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45853.291666666664</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45853.666666666664</v>
+      </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="9">
+        <v>45839.291666666664</v>
+      </c>
+      <c r="C17" s="9">
+        <v>45839.666666666664</v>
+      </c>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="9">
+        <v>45840.291666666664</v>
+      </c>
+      <c r="C18" s="9">
+        <v>45840.666666666664</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="9">
+        <v>45841.291666666664</v>
+      </c>
+      <c r="C19" s="9">
+        <v>45841.666666666664</v>
+      </c>
       <c r="D19" s="1"/>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="9">
+        <v>45842.291666666664</v>
+      </c>
+      <c r="C20" s="9">
+        <v>45842.666666666664</v>
+      </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="1"/>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="9">
+        <v>45843.291666666664</v>
+      </c>
+      <c r="C21" s="9">
+        <v>45843.666666666664</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="9">
+        <v>45844.291666666664</v>
+      </c>
+      <c r="C22" s="9">
+        <v>45844.666666666664</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="9">
+        <v>45845.291666666664</v>
+      </c>
+      <c r="C23" s="9">
+        <v>45845.666666666664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="9">
+        <v>45846.291666666664</v>
+      </c>
+      <c r="C24" s="9">
+        <v>45846.666666666664</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="9">
+        <v>45847.291666666664</v>
+      </c>
+      <c r="C25" s="9">
+        <v>45847.666666666664</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="9">
+        <v>45848.291666666664</v>
+      </c>
+      <c r="C26" s="9">
+        <v>45848.666666666664</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="9">
+        <v>45849.291666666664</v>
+      </c>
+      <c r="C27" s="9">
+        <v>45849.666666666664</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="9">
+        <v>45850.291666666664</v>
+      </c>
+      <c r="C28" s="9">
+        <v>45850.666666666664</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="9">
+        <v>45851.291666666664</v>
+      </c>
+      <c r="C29" s="9">
+        <v>45851.666666666664</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="9">
+        <v>45852.291666666664</v>
+      </c>
+      <c r="C30" s="9">
+        <v>45852.666666666664</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="9">
+        <v>45853.291666666664</v>
+      </c>
+      <c r="C31" s="9">
+        <v>45853.666666666664</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="9">
+        <v>45839.291666666664</v>
+      </c>
+      <c r="C32" s="9">
+        <v>45839.666666666664</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="9">
+        <v>45840.291666608799</v>
+      </c>
+      <c r="C33" s="9">
+        <v>45840.666666608799</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" s="9">
+        <v>45841.291666608799</v>
+      </c>
+      <c r="C34" s="9">
+        <v>45841.666666608799</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="9">
+        <v>45842.291666608799</v>
+      </c>
+      <c r="C35" s="9">
+        <v>45842.666666608799</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" s="9">
+        <v>45843.291666608799</v>
+      </c>
+      <c r="C36" s="9">
+        <v>45843.666666608799</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="9">
+        <v>45844.291666608799</v>
+      </c>
+      <c r="C37" s="9">
+        <v>45844.666666608799</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" s="9">
+        <v>45845.291666608799</v>
+      </c>
+      <c r="C38" s="9">
+        <v>45845.666666608799</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" s="9">
+        <v>45846.291666608799</v>
+      </c>
+      <c r="C39" s="9">
+        <v>45846.666666608799</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" s="9">
+        <v>45847.291666608799</v>
+      </c>
+      <c r="C40" s="9">
+        <v>45847.666666608799</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="9">
+        <v>45848.291666608799</v>
+      </c>
+      <c r="C41" s="9">
+        <v>45848.666666608799</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" s="9">
+        <v>45849.291666608799</v>
+      </c>
+      <c r="C42" s="9">
+        <v>45849.666666608799</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="9">
+        <v>45850.291666608799</v>
+      </c>
+      <c r="C43" s="9">
+        <v>45850.666666608799</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="9">
+        <v>45851.291666608799</v>
+      </c>
+      <c r="C44" s="9">
+        <v>45851.666666608799</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" s="9">
+        <v>45852.291666608799</v>
+      </c>
+      <c r="C45" s="9">
+        <v>45852.666666608799</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="9">
+        <v>45853.291666608799</v>
+      </c>
+      <c r="C46" s="9">
+        <v>45853.666666608799</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -682,4 +1014,394 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FCB5A7-0D53-451A-9903-54FB04400900}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.86328125" customWidth="1"/>
+    <col min="2" max="3" width="18.19921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9">
+        <v>45839.291666666664</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45839.666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="9">
+        <v>45840.291666666664</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45840.666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <v>45841.291666666664</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45841.666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>45842.291666666664</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45842.666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>45843.291666666664</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45843.666666666664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9">
+        <v>45844.291666666664</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45844.666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9">
+        <v>45845.291666666664</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45845.666666666664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="9">
+        <v>45846.291666666664</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45846.666666666664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45847.291666666664</v>
+      </c>
+      <c r="C10" s="9">
+        <v>45847.666666666664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45848.291666666664</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45848.666666666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45849.291666666664</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45849.666666666664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45850.291666666664</v>
+      </c>
+      <c r="C13" s="9">
+        <v>45850.666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45851.291666666664</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45851.666666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45852.291666666664</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45852.666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45853.291666666664</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45853.666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDDACE2A-BE0F-4A72-BC4F-3E22BAF571DB}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="2" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="9">
+        <v>45839.291666666664</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45839.666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="9">
+        <v>45840.291666666664</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45840.666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="9">
+        <v>45841.291666666664</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45841.666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="9">
+        <v>45842.291666666664</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45842.666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="9">
+        <v>45843.291666666664</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45843.666666666664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>45844.291666666664</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45844.666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9">
+        <v>45845.291666666664</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45845.666666666664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9">
+        <v>45846.291666666664</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45846.666666666664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45847.291666666664</v>
+      </c>
+      <c r="C10" s="9">
+        <v>45847.666666666664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45848.291666666664</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45848.666666666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45849.291666666664</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45849.666666666664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45850.291666666664</v>
+      </c>
+      <c r="C13" s="9">
+        <v>45850.666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45851.291666666664</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45851.666666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45852.291666666664</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45852.666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45853.291666666664</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45853.666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
reporte de planilla columnas faltantes
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
+++ b/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_retenciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8842F636-8194-46D3-BC97-231CCD65EA23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095E2FCB-7500-4A84-B740-11FC14530073}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencia" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja2" sheetId="3" r:id="rId3"/>
+    <sheet name="AGOSto" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="7">
   <si>
     <t>Empleado</t>
   </si>
@@ -36,13 +37,13 @@
     <t>Karen Burgos</t>
   </si>
   <si>
-    <t>Tina Williamson</t>
-  </si>
-  <si>
     <t>Arely siguenza</t>
   </si>
   <si>
     <t>Adriana Díaz</t>
+  </si>
+  <si>
+    <t>Sharlene Rhodes</t>
   </si>
 </sst>
 </file>
@@ -52,7 +53,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy\ hh:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
+    <numFmt numFmtId="166" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -113,7 +114,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -420,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -454,7 +455,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="9">
-        <v>45839.291666666664</v>
+        <v>45854.291666666664</v>
       </c>
       <c r="C2" s="9">
         <v>45839.666666666664</v>
@@ -469,7 +470,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="9">
-        <v>45840.291666666664</v>
+        <v>45855.291666666664</v>
       </c>
       <c r="C3" s="9">
         <v>45840.666666666664</v>
@@ -484,7 +485,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9">
-        <v>45841.291666666664</v>
+        <v>45856.291666666664</v>
       </c>
       <c r="C4" s="9">
         <v>45841.666666666664</v>
@@ -499,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="9">
-        <v>45842.291666666664</v>
+        <v>45857.291666666664</v>
       </c>
       <c r="C5" s="9">
         <v>45842.666666666664</v>
@@ -514,7 +515,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="9">
-        <v>45843.291666666664</v>
+        <v>45858.291666666664</v>
       </c>
       <c r="C6" s="9">
         <v>45843.666666666664</v>
@@ -529,7 +530,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="9">
-        <v>45844.291666666664</v>
+        <v>45859.291666666664</v>
       </c>
       <c r="C7" s="9">
         <v>45844.666666666664</v>
@@ -544,7 +545,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="9">
-        <v>45845.291666666664</v>
+        <v>45860.291666666664</v>
       </c>
       <c r="C8" s="9">
         <v>45845.666666666664</v>
@@ -559,7 +560,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="9">
-        <v>45846.291666666664</v>
+        <v>45861.291666666664</v>
       </c>
       <c r="C9" s="9">
         <v>45846.666666666664</v>
@@ -574,7 +575,7 @@
         <v>3</v>
       </c>
       <c r="B10" s="9">
-        <v>45847.291666666664</v>
+        <v>45862.291666666664</v>
       </c>
       <c r="C10" s="9">
         <v>45847.666666666664</v>
@@ -589,7 +590,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="9">
-        <v>45848.291666666664</v>
+        <v>45863.291666666664</v>
       </c>
       <c r="C11" s="9">
         <v>45848.666666666664</v>
@@ -604,7 +605,7 @@
         <v>3</v>
       </c>
       <c r="B12" s="9">
-        <v>45849.291666666664</v>
+        <v>45864.291666608799</v>
       </c>
       <c r="C12" s="9">
         <v>45849.666666666664</v>
@@ -619,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="B13" s="9">
-        <v>45850.291666666664</v>
+        <v>45865.291666608799</v>
       </c>
       <c r="C13" s="9">
         <v>45850.666666666664</v>
@@ -634,7 +635,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="9">
-        <v>45851.291666666664</v>
+        <v>45866.291666608799</v>
       </c>
       <c r="C14" s="9">
         <v>45851.666666666664</v>
@@ -649,7 +650,7 @@
         <v>3</v>
       </c>
       <c r="B15" s="9">
-        <v>45852.291666666664</v>
+        <v>45867.291666608799</v>
       </c>
       <c r="C15" s="9">
         <v>45852.666666666664</v>
@@ -661,7 +662,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="9">
-        <v>45853.291666666664</v>
+        <v>45868.291666608799</v>
       </c>
       <c r="C16" s="9">
         <v>45853.666666666664</v>
@@ -669,336 +670,342 @@
       <c r="D16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="9">
-        <v>45839.291666666664</v>
-      </c>
-      <c r="C17" s="9">
-        <v>45839.666666666664</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="B17" s="9"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="1"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B18" s="9">
-        <v>45840.291666666664</v>
+        <v>45839.291666666664</v>
       </c>
       <c r="C18" s="9">
-        <v>45840.666666666664</v>
+        <v>45839.666666666664</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B19" s="9">
-        <v>45841.291666666664</v>
+        <v>45840.291666666664</v>
       </c>
       <c r="C19" s="9">
-        <v>45841.666666666664</v>
+        <v>45840.666666666664</v>
       </c>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" s="9">
-        <v>45842.291666666664</v>
+        <v>45841.291666666664</v>
       </c>
       <c r="C20" s="9">
-        <v>45842.666666666664</v>
+        <v>45841.666666666664</v>
       </c>
       <c r="D20" s="1"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B21" s="9">
-        <v>45843.291666666664</v>
+        <v>45842.291666666664</v>
       </c>
       <c r="C21" s="9">
-        <v>45843.666666666664</v>
-      </c>
+        <v>45842.666666666664</v>
+      </c>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B22" s="9">
-        <v>45844.291666666664</v>
+        <v>45843.291666666664</v>
       </c>
       <c r="C22" s="9">
-        <v>45844.666666666664</v>
+        <v>45843.666666666664</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B23" s="9">
-        <v>45845.291666666664</v>
+        <v>45844.291666666664</v>
       </c>
       <c r="C23" s="9">
-        <v>45845.666666666664</v>
+        <v>45844.666666666664</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" s="9">
-        <v>45846.291666666664</v>
+        <v>45845.291666666664</v>
       </c>
       <c r="C24" s="9">
-        <v>45846.666666666664</v>
+        <v>45845.666666666664</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" s="9">
-        <v>45847.291666666664</v>
+        <v>45846.291666666664</v>
       </c>
       <c r="C25" s="9">
-        <v>45847.666666666664</v>
+        <v>45846.666666666664</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="9">
-        <v>45848.291666666664</v>
+        <v>45847.291666666664</v>
       </c>
       <c r="C26" s="9">
-        <v>45848.666666666664</v>
+        <v>45847.666666666664</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B27" s="9">
-        <v>45849.291666666664</v>
+        <v>45848.291666666664</v>
       </c>
       <c r="C27" s="9">
-        <v>45849.666666666664</v>
+        <v>45848.666666666664</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28" s="9">
-        <v>45850.291666666664</v>
+        <v>45849.291666666664</v>
       </c>
       <c r="C28" s="9">
-        <v>45850.666666666664</v>
+        <v>45849.666666666664</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B29" s="9">
-        <v>45851.291666666664</v>
+        <v>45850.291666666664</v>
       </c>
       <c r="C29" s="9">
-        <v>45851.666666666664</v>
+        <v>45850.666666666664</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B30" s="9">
+        <v>45851.291666666664</v>
+      </c>
+      <c r="C30" s="9">
+        <v>45851.666666666664</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="9">
         <v>45852.291666666664</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C31" s="9">
         <v>45852.666666666664</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B31" s="9">
+    <row r="32" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="9">
         <v>45853.291666666664</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C32" s="9">
         <v>45853.666666666664</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>6</v>
-      </c>
-      <c r="B32" s="9">
-        <v>45839.291666666664</v>
-      </c>
-      <c r="C32" s="9">
-        <v>45839.666666666664</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B33" s="9">
-        <v>45840.291666608799</v>
+        <v>45839.291666666664</v>
       </c>
       <c r="C33" s="9">
-        <v>45840.666666608799</v>
+        <v>45839.666666666664</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B34" s="9">
-        <v>45841.291666608799</v>
+        <v>45840.291666608799</v>
       </c>
       <c r="C34" s="9">
-        <v>45841.666666608799</v>
+        <v>45840.666666608799</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B35" s="9">
-        <v>45842.291666608799</v>
+        <v>45841.291666608799</v>
       </c>
       <c r="C35" s="9">
-        <v>45842.666666608799</v>
+        <v>45841.666666608799</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B36" s="9">
-        <v>45843.291666608799</v>
+        <v>45842.291666608799</v>
       </c>
       <c r="C36" s="9">
-        <v>45843.666666608799</v>
+        <v>45842.666666608799</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B37" s="9">
-        <v>45844.291666608799</v>
+        <v>45843.291666608799</v>
       </c>
       <c r="C37" s="9">
-        <v>45844.666666608799</v>
+        <v>45843.666666608799</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B38" s="9">
-        <v>45845.291666608799</v>
+        <v>45844.291666608799</v>
       </c>
       <c r="C38" s="9">
-        <v>45845.666666608799</v>
+        <v>45844.666666608799</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B39" s="9">
-        <v>45846.291666608799</v>
+        <v>45845.291666608799</v>
       </c>
       <c r="C39" s="9">
-        <v>45846.666666608799</v>
+        <v>45845.666666608799</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B40" s="9">
-        <v>45847.291666608799</v>
+        <v>45846.291666608799</v>
       </c>
       <c r="C40" s="9">
-        <v>45847.666666608799</v>
+        <v>45846.666666608799</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B41" s="9">
-        <v>45848.291666608799</v>
+        <v>45847.291666608799</v>
       </c>
       <c r="C41" s="9">
-        <v>45848.666666608799</v>
+        <v>45847.666666608799</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B42" s="9">
-        <v>45849.291666608799</v>
+        <v>45848.291666608799</v>
       </c>
       <c r="C42" s="9">
-        <v>45849.666666608799</v>
+        <v>45848.666666608799</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B43" s="9">
-        <v>45850.291666608799</v>
+        <v>45849.291666608799</v>
       </c>
       <c r="C43" s="9">
-        <v>45850.666666608799</v>
+        <v>45849.666666608799</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44" s="9">
-        <v>45851.291666608799</v>
+        <v>45850.291666608799</v>
       </c>
       <c r="C44" s="9">
-        <v>45851.666666608799</v>
+        <v>45850.666666608799</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B45" s="9">
-        <v>45852.291666608799</v>
+        <v>45851.291666608799</v>
       </c>
       <c r="C45" s="9">
-        <v>45852.666666608799</v>
+        <v>45851.666666608799</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B46" s="9">
+        <v>45852.291666608799</v>
+      </c>
+      <c r="C46" s="9">
+        <v>45852.666666608799</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="9">
         <v>45853.291666608799</v>
       </c>
-      <c r="C46" s="9">
+      <c r="C47" s="9">
         <v>45853.666666608799</v>
       </c>
     </row>
@@ -1020,8 +1027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7FCB5A7-0D53-451A-9903-54FB04400900}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:C16"/>
+    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1043,7 +1050,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B2" s="9">
         <v>45839.291666666664</v>
@@ -1054,7 +1061,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" s="9">
         <v>45840.291666666664</v>
@@ -1065,7 +1072,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" s="9">
         <v>45841.291666666664</v>
@@ -1076,7 +1083,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5" s="9">
         <v>45842.291666666664</v>
@@ -1087,7 +1094,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6" s="9">
         <v>45843.291666666664</v>
@@ -1098,7 +1105,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B7" s="9">
         <v>45844.291666666664</v>
@@ -1109,7 +1116,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B8" s="9">
         <v>45845.291666666664</v>
@@ -1120,7 +1127,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B9" s="9">
         <v>45846.291666666664</v>
@@ -1131,7 +1138,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B10" s="9">
         <v>45847.291666666664</v>
@@ -1142,7 +1149,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B11" s="9">
         <v>45848.291666666664</v>
@@ -1153,7 +1160,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B12" s="9">
         <v>45849.291666666664</v>
@@ -1164,7 +1171,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B13" s="9">
         <v>45850.291666666664</v>
@@ -1175,7 +1182,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" s="9">
         <v>45851.291666666664</v>
@@ -1186,7 +1193,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B15" s="9">
         <v>45852.291666666664</v>
@@ -1197,7 +1204,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" s="9">
         <v>45853.291666666664</v>
@@ -1238,7 +1245,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="9">
         <v>45839.291666666664</v>
@@ -1249,7 +1256,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" s="9">
         <v>45840.291666666664</v>
@@ -1260,7 +1267,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9">
         <v>45841.291666666664</v>
@@ -1271,7 +1278,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="9">
         <v>45842.291666666664</v>
@@ -1282,7 +1289,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="9">
         <v>45843.291666666664</v>
@@ -1293,7 +1300,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="9">
         <v>45844.291666666664</v>
@@ -1304,7 +1311,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="9">
         <v>45845.291666666664</v>
@@ -1315,7 +1322,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" s="9">
         <v>45846.291666666664</v>
@@ -1326,7 +1333,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" s="9">
         <v>45847.291666666664</v>
@@ -1337,7 +1344,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="9">
         <v>45848.291666666664</v>
@@ -1348,7 +1355,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" s="9">
         <v>45849.291666666664</v>
@@ -1359,7 +1366,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B13" s="9">
         <v>45850.291666666664</v>
@@ -1370,7 +1377,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="9">
         <v>45851.291666666664</v>
@@ -1381,7 +1388,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B15" s="9">
         <v>45852.291666666664</v>
@@ -1392,13 +1399,219 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="9">
         <v>45853.291666666664</v>
       </c>
       <c r="C16" s="9">
         <v>45853.666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6104F2-018B-4BC2-A48B-A93F265BC1F3}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" customWidth="1"/>
+    <col min="2" max="3" width="17.796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9">
+        <v>45854.291666666664</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45854.666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>45855.291666666664</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45855.666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9">
+        <v>45856.291666666664</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45856.666666608799</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="9">
+        <v>45857.291666666664</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45857.666666608799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>45858.291666666664</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45858.666666608799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9">
+        <v>45859.291666666664</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45859.666666608799</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="9">
+        <v>45860.291666666664</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45860.666666608799</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="9">
+        <v>45861.291666666664</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45861.666666608799</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45862.291666666664</v>
+      </c>
+      <c r="C10" s="9">
+        <v>45862.666666608799</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45863.291666666664</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45863.666666608799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45864.291666608799</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45864.666666608799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45865.291666608799</v>
+      </c>
+      <c r="C13" s="9">
+        <v>45865.666666608799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45866.291666608799</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45866.666666608799</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45867.291666608799</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45867.666666608799</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45868.291666608799</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45868.666666608799</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="9">
+        <v>45869.291666608799</v>
+      </c>
+      <c r="C17" s="9">
+        <v>45869.666666608799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
separacion de tipos de afp en reportes y recibo de nomina
</commit_message>
<xml_diff>
--- a/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
+++ b/location/l10n_sv_hr_retenciones/static/src/plantilla/plantilla_asistencia.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Documents\GitHub\fe\location\l10n_sv_hr_retenciones\static\src\plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA622B4-F5FF-4EFE-A5EA-8978E945E4A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEC27731-7CF1-41BF-8281-7AF0D19423F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Asistencia (2)" sheetId="5" r:id="rId1"/>
     <sheet name="Asistencia Q2 julio" sheetId="1" r:id="rId2"/>
     <sheet name="Asistencia Q1 Agosto" sheetId="6" r:id="rId3"/>
+    <sheet name="Asistencia Q1 Agosto (2)" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="7">
   <si>
     <t>Empleado</t>
   </si>
@@ -40,6 +41,9 @@
   </si>
   <si>
     <t>Adriana Díaz</t>
+  </si>
+  <si>
+    <t>Ana Flores</t>
   </si>
 </sst>
 </file>
@@ -683,7 +687,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C1" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
@@ -1310,7 +1314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F4A3153-0111-4C7E-BDCB-FC801DDB6CB7}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C17" sqref="C17:C31"/>
     </sheetView>
   </sheetViews>
@@ -1664,4 +1668,199 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FBBA87A-4FBD-4A5B-A7DF-F5D34E3BEA6D}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.59765625" customWidth="1"/>
+    <col min="2" max="3" width="19.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="9">
+        <v>45870.291666666664</v>
+      </c>
+      <c r="C2" s="9">
+        <v>45870.666666666664</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="9">
+        <v>45871.291666666664</v>
+      </c>
+      <c r="C3" s="9">
+        <v>45871.666666666664</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="9">
+        <v>45872.291666666664</v>
+      </c>
+      <c r="C4" s="9">
+        <v>45872.666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="9">
+        <v>45873.291666666664</v>
+      </c>
+      <c r="C5" s="9">
+        <v>45873.666666666664</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="9">
+        <v>45874.291666666664</v>
+      </c>
+      <c r="C6" s="9">
+        <v>45874.666666666664</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="9">
+        <v>45875.291666666664</v>
+      </c>
+      <c r="C7" s="9">
+        <v>45875.666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="9">
+        <v>45876.291666666664</v>
+      </c>
+      <c r="C8" s="9">
+        <v>45876.666666666664</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9">
+        <v>45877.291666666664</v>
+      </c>
+      <c r="C9" s="9">
+        <v>45877.666666666664</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="9">
+        <v>45878.291666666664</v>
+      </c>
+      <c r="C10" s="9">
+        <v>45878.666666666664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="9">
+        <v>45879.291666666664</v>
+      </c>
+      <c r="C11" s="9">
+        <v>45879.666666666664</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="9">
+        <v>45880.291666666664</v>
+      </c>
+      <c r="C12" s="9">
+        <v>45880.666666666664</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="9">
+        <v>45881.291666666664</v>
+      </c>
+      <c r="C13" s="9">
+        <v>45881.666666666664</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="9">
+        <v>45882.291666666664</v>
+      </c>
+      <c r="C14" s="9">
+        <v>45882.666666666664</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="9">
+        <v>45883.291666666664</v>
+      </c>
+      <c r="C15" s="9">
+        <v>45883.666666666664</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="9">
+        <v>45884.291666666664</v>
+      </c>
+      <c r="C16" s="9">
+        <v>45884.666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>